<commit_message>
Aula 02 - Formatação da Planilha Início
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -292,6 +292,260 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>574632</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4162425" cy="843693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4337007" y="1133475"/>
+          <a:ext cx="4162425" cy="843693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2400" b="1">
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>CONTROLE DE ESTOQUES SIMPLIFICADO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>805365</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5796459" cy="1203856"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CaixaDeTexto 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3519990" y="2466975"/>
+          <a:ext cx="5796459" cy="1203856"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1">
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ORIENTAÇÕES</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1. Cadastrar o produto na aba "Cadastro".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>2. Registrar as entradas e saídas na aba "Lançamentos".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>3. Relatórios e consultas usar os filtros nas abas "Cadastro" e "Lançamentos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>".</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1200">
+            <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2267712</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2199513" cy="564706"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CaixaDeTexto 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10221087" y="0"/>
+          <a:ext cx="2199513" cy="564706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Douglas Barros Nery</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1"/>
+            <a:t>Controle de Estoque</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1034,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,6 +1304,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1057,7 +1312,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -1080,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 03 - Criação das Tabelas
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -4,23 +4,93 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="7" r:id="rId2"/>
     <sheet name="Lançamentos" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+  <si>
+    <t>PRODUTO</t>
+  </si>
+  <si>
+    <t>MEDIDA</t>
+  </si>
+  <si>
+    <t>ESTOQUE
+MÍNIMO</t>
+  </si>
+  <si>
+    <t>SALDO</t>
+  </si>
+  <si>
+    <t>AVISOS</t>
+  </si>
+  <si>
+    <t>Caneta esferográfica azul</t>
+  </si>
+  <si>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>ESTOQUE
+MÁXIMO</t>
+  </si>
+  <si>
+    <t>Caneta esferográfica preta</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>ENTRADA</t>
+  </si>
+  <si>
+    <t>SAÍDA</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -52,15 +122,371 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="EstiloTabelaPersonalizado" pivot="0" count="0"/>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF008000"/>
+      <color rgb="FF006600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -772,6 +1198,74 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2266950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2199513" cy="564706"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10220325" y="0"/>
+          <a:ext cx="2199513" cy="564706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Douglas Barros Nery</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1"/>
+            <a:t>Controle de Estoque</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -998,7 +1492,104 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2266950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2199513" cy="564706"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10220325" y="0"/>
+          <a:ext cx="2199513" cy="564706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Douglas Barros Nery</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1400"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1"/>
+            <a:t>Controle de Estoque</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="42" totalsRowDxfId="41">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="ESTOQUE_x000a_MÍNIMO" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="ESTOQUE_x000a_MÁXIMO" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="SALDO" dataDxfId="40" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="39" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E6" totalsRowCount="1" headerRowDxfId="28" totalsRowDxfId="27">
+  <autoFilter ref="A3:E5"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="24" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="7"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1290,7 +1881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1304,7 +1895,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1312,10 +1903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,19 +1917,99 @@
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>150</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <f>SUBTOTAL(103,TblCadastro[AVISOS])</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A4:D5">
+    <cfRule type="expression" dxfId="11" priority="1">
+      <formula>ODD(ROW())=ROW()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D5">
+      <formula1>0</formula1>
+      <formula2>1000000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,9 +2020,95 @@
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>43698</v>
+      </c>
+      <c r="C4" s="5">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>43699</v>
+      </c>
+      <c r="C5" s="5">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <f>SUBTOTAL(103,TblLancamentos[DATA])</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <f>SUBTOTAL(109,TblLancamentos[ENTRADA])</f>
+        <v>50</v>
+      </c>
+      <c r="D6" s="6">
+        <f>SUBTOTAL(109,TblLancamentos[SAÍDA])</f>
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <f>SUBTOTAL(103,TblLancamentos[SALDO])</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A4:D5">
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>ODD(ROW())=ROW()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B5">
+      <formula1>1</formula1>
+      <formula2>401769</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D5">
+      <formula1>0</formula1>
+      <formula2>1000000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aula 04 - Lista de validação usando caixa de nome
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
     <sheet name="Cadastro" sheetId="7" r:id="rId2"/>
     <sheet name="Lançamentos" sheetId="6" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="ColunaProdutos">TblCadastro[PRODUTO]</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -1905,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2098,7 @@
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B5">
       <formula1>1</formula1>
       <formula2>401769</formula2>
@@ -2103,6 +2106,9 @@
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D5">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A5">
+      <formula1>ColunaProdutos</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aula 05 - Saldo de produtos com SOMASE
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>PRODUTO</t>
   </si>
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,13 @@
       <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -137,18 +144,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -158,6 +165,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -166,179 +174,11 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -372,7 +212,6 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -403,48 +242,105 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -1567,29 +1463,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="42" totalsRowDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="24" totalsRowDxfId="23">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="ESTOQUE_x000a_MÍNIMO" totalsRowDxfId="3"/>
-    <tableColumn id="4" name="ESTOQUE_x000a_MÁXIMO" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="SALDO" dataDxfId="40" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="39" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="20"/>
+    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="19"/>
+    <tableColumn id="3" name="ESTOQUE_x000a_MÍNIMO" totalsRowDxfId="18"/>
+    <tableColumn id="4" name="ESTOQUE_x000a_MÁXIMO" totalsRowDxfId="17"/>
+    <tableColumn id="5" name="SALDO" dataDxfId="21" totalsRowDxfId="16">
+      <calculatedColumnFormula>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="22" totalsRowDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E6" totalsRowCount="1" headerRowDxfId="28" totalsRowDxfId="27">
-  <autoFilter ref="A3:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E7" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="13">
+  <autoFilter ref="A3:E6"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="24" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="12"/>
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1908,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1852,10 @@
       <c r="D4">
         <v>150</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>35</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1970,7 +1871,10 @@
       <c r="D5">
         <v>150</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>48</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1988,7 +1892,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:D5">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2009,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,10 +1935,10 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -2072,42 +1976,57 @@
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43605</v>
+      </c>
+      <c r="C6" s="5">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <f>SUBTOTAL(103,TblLancamentos[DATA])</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
         <f>SUBTOTAL(109,TblLancamentos[ENTRADA])</f>
-        <v>50</v>
-      </c>
-      <c r="D6" s="6">
+        <v>100</v>
+      </c>
+      <c r="D7" s="6">
         <f>SUBTOTAL(109,TblLancamentos[SAÍDA])</f>
-        <v>15</v>
-      </c>
-      <c r="E6" s="1">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1">
         <f>SUBTOTAL(103,TblLancamentos[SALDO])</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:D5">
-    <cfRule type="expression" dxfId="10" priority="1">
+  <conditionalFormatting sqref="A4:D6">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B5">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B6">
       <formula1>1</formula1>
       <formula2>401769</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D5">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D6">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6">
       <formula1>ColunaProdutos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Aula 06 - Saldo de produtos com SOMASES
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>PRODUTO</t>
   </si>
@@ -301,6 +301,14 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
@@ -308,6 +316,15 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -334,23 +351,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
@@ -1466,28 +1466,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="24" totalsRowDxfId="23">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="20"/>
-    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="19"/>
-    <tableColumn id="3" name="ESTOQUE_x000a_MÍNIMO" totalsRowDxfId="18"/>
-    <tableColumn id="4" name="ESTOQUE_x000a_MÁXIMO" totalsRowDxfId="17"/>
-    <tableColumn id="5" name="SALDO" dataDxfId="21" totalsRowDxfId="16">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="22"/>
+    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="21"/>
+    <tableColumn id="3" name="ESTOQUE_x000a_MÍNIMO" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="ESTOQUE_x000a_MÁXIMO" totalsRowDxfId="19"/>
+    <tableColumn id="5" name="SALDO" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="22" totalsRowDxfId="15"/>
+    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E7" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="13">
-  <autoFilter ref="A3:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="13">
+  <autoFilter ref="A3:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="4"/>
     <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="3"/>
     <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="2"/>
     <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="0"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="0">
+      <calculatedColumnFormula>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1806,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1875,7 @@
       </c>
       <c r="E5" s="1">
         <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1913,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,7 +1960,10 @@
       <c r="D4" s="5">
         <v>5</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="6">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1973,7 +1978,10 @@
       <c r="D5" s="5">
         <v>10</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1988,45 +1996,66 @@
       <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43497</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <f>SUBTOTAL(103,TblLancamentos[DATA])</f>
-        <v>3</v>
-      </c>
-      <c r="C7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6">
         <f>SUBTOTAL(109,TblLancamentos[ENTRADA])</f>
-        <v>100</v>
-      </c>
-      <c r="D7" s="6">
+        <v>110</v>
+      </c>
+      <c r="D8" s="6">
         <f>SUBTOTAL(109,TblLancamentos[SAÍDA])</f>
-        <v>17</v>
-      </c>
-      <c r="E7" s="1">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
         <f>SUBTOTAL(103,TblLancamentos[SALDO])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:D6">
+  <conditionalFormatting sqref="A4:D7">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B6">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B7">
       <formula1>1</formula1>
       <formula2>401769</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D7">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A7">
       <formula1>ColunaProdutos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Aula 07 - Avisos utilizando a fórmula SE
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,6 @@
     <t>MEDIDA</t>
   </si>
   <si>
-    <t>ESTOQUE
-MÍNIMO</t>
-  </si>
-  <si>
     <t>SALDO</t>
   </si>
   <si>
@@ -41,10 +37,6 @@
   </si>
   <si>
     <t>Unidade</t>
-  </si>
-  <si>
-    <t>ESTOQUE
-MÁXIMO</t>
   </si>
   <si>
     <t>Caneta esferográfica preta</t>
@@ -60,6 +52,12 @@
   </si>
   <si>
     <t>SAÍDA</t>
+  </si>
+  <si>
+    <t>ESTOQUE MÍNIMO</t>
+  </si>
+  <si>
+    <t>ESTOQUE MÁXIMO</t>
   </si>
 </sst>
 </file>
@@ -155,7 +153,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -215,29 +213,58 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
     </dxf>
@@ -293,25 +320,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -319,38 +329,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
@@ -375,6 +353,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
@@ -806,7 +791,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2267712</xdr:colOff>
+      <xdr:colOff>1848612</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -818,7 +803,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10221087" y="0"/>
+          <a:off x="10268712" y="0"/>
           <a:ext cx="2199513" cy="564706"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1100,7 +1085,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2266950</xdr:colOff>
+      <xdr:colOff>1848612</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1112,7 +1097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10220325" y="0"/>
+          <a:off x="10268712" y="0"/>
           <a:ext cx="2199513" cy="564706"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1394,7 +1379,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2266950</xdr:colOff>
+      <xdr:colOff>1848612</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1406,7 +1391,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10220325" y="0"/>
+          <a:off x="10268712" y="0"/>
           <a:ext cx="2199513" cy="564706"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1463,31 +1448,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="24" totalsRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="21" totalsRowDxfId="20">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="22"/>
-    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="21"/>
-    <tableColumn id="3" name="ESTOQUE_x000a_MÍNIMO" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="ESTOQUE_x000a_MÁXIMO" totalsRowDxfId="19"/>
-    <tableColumn id="5" name="SALDO" dataDxfId="18" totalsRowDxfId="17">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="10"/>
+    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="ESTOQUE MÍNIMO" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="ESTOQUE MÁXIMO" totalsRowDxfId="7"/>
+    <tableColumn id="5" name="SALDO" dataDxfId="19" totalsRowDxfId="6">
       <calculatedColumnFormula>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="5">
+      <calculatedColumnFormula>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="EstiloTabelaPersonalizado" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="17" totalsRowDxfId="16">
   <autoFilter ref="A3:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="0">
+    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="0">
       <calculatedColumnFormula>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1784,15 +1771,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="67" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -1808,15 +1796,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="67" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -1829,24 +1818,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -1856,16 +1845,19 @@
       </c>
       <c r="E4" s="1">
         <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
-        <v>35</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>998</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v>Priorizar venda!</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -1875,13 +1867,16 @@
       </c>
       <c r="E5" s="1">
         <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
-        <v>46</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>-9952</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v>Solicitar nova compra!</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1889,12 +1884,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <f>SUBTOTAL(103,TblCadastro[AVISOS])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:D5">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1917,15 +1912,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="67" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -1935,39 +1931,39 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>43698</v>
       </c>
       <c r="C4" s="5">
-        <v>30</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="5">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>25</v>
+        <v>988</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>43699</v>
@@ -1980,12 +1976,12 @@
       </c>
       <c r="E5" s="6">
         <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>35</v>
+        <v>998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
         <v>43605</v>
@@ -1994,16 +1990,16 @@
         <v>50</v>
       </c>
       <c r="D6" s="5">
-        <v>2</v>
+        <v>10000</v>
       </c>
       <c r="E6" s="6">
         <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>46</v>
+        <v>-9952</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>43497</v>
@@ -2021,7 +2017,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <f>SUBTOTAL(103,TblLancamentos[DATA])</f>
@@ -2029,11 +2025,11 @@
       </c>
       <c r="C8" s="6">
         <f>SUBTOTAL(109,TblLancamentos[ENTRADA])</f>
-        <v>110</v>
+        <v>1080</v>
       </c>
       <c r="D8" s="6">
         <f>SUBTOTAL(109,TblLancamentos[SAÍDA])</f>
-        <v>29</v>
+        <v>10034</v>
       </c>
       <c r="E8" s="1">
         <f>SUBTOTAL(103,TblLancamentos[SALDO])</f>
@@ -2042,7 +2038,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:D7">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Aula 08 - Formatação condicional para destacar informações
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,13 +94,6 @@
       <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -148,12 +141,76 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -212,59 +269,21 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -319,11 +338,179 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFF66"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -335,6 +522,15 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -353,13 +549,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
@@ -367,6 +556,8 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFFFF99"/>
       <color rgb="FF008000"/>
       <color rgb="FF006600"/>
     </mruColors>
@@ -1448,17 +1639,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="21" totalsRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="45" totalsRowDxfId="44">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="10"/>
-    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="ESTOQUE MÍNIMO" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="ESTOQUE MÁXIMO" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="SALDO" dataDxfId="19" totalsRowDxfId="6">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="26"/>
+    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="25"/>
+    <tableColumn id="3" name="ESTOQUE MÍNIMO" totalsRowDxfId="24"/>
+    <tableColumn id="4" name="ESTOQUE MÁXIMO" totalsRowDxfId="23"/>
+    <tableColumn id="5" name="SALDO" dataDxfId="43" totalsRowDxfId="22">
       <calculatedColumnFormula>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="5">
+    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="42" totalsRowDxfId="21">
       <calculatedColumnFormula>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1467,14 +1658,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="19" totalsRowDxfId="18">
   <autoFilter ref="A3:E7"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="0">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="10"/>
+    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="8"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="7">
       <calculatedColumnFormula>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1797,7 +1988,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,8 +2080,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:D5">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>ODD(ROW())=ROW()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F5">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Priorizar venda!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>"Solicitar nova compra!"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1913,7 +2112,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,8 +2237,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:D7">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ODD(ROW())=ROW()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">

</xml_diff>

<commit_message>
Aula 09 - Criação do gráfico
</commit_message>
<xml_diff>
--- a/Projeto-Controle-Estoque.xlsx
+++ b/Projeto-Controle-Estoque.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="20">
   <si>
     <t>PRODUTO</t>
   </si>
@@ -59,12 +59,33 @@
   <si>
     <t>ESTOQUE MÁXIMO</t>
   </si>
+  <si>
+    <t>Caneta esferográfica vermelha</t>
+  </si>
+  <si>
+    <t>Cola branca 90ml</t>
+  </si>
+  <si>
+    <t>Lápis preto # 2</t>
+  </si>
+  <si>
+    <t>Caixa</t>
+  </si>
+  <si>
+    <t>Lapiseira 0,5mm</t>
+  </si>
+  <si>
+    <t>Lapiseira 0,7mm</t>
+  </si>
+  <si>
+    <t>Lapiseira 0,9mm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +117,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -123,14 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -141,76 +174,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFFF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -238,12 +218,30 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -272,40 +270,18 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -351,11 +327,34 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -364,6 +363,31 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -372,44 +396,152 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -437,119 +569,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFFF66"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="EstiloTabelaPersonalizado" pivot="0" count="0"/>
@@ -568,6 +587,166 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Cadastro!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SALDO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1300" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Cadastro!$A$4:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Caneta esferográfica azul</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Caneta esferográfica preta</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Caneta esferográfica vermelha</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cola branca 90ml</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lápis preto # 2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Lapiseira 0,5mm</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Lapiseira 0,7mm</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lapiseira 0,9mm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Cadastro!$E$4:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="45"/>
+      </c:doughnutChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1341,6 +1520,101 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3962400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3857625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CaixaDeTexto 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8667750" y="714375"/>
+          <a:ext cx="3609975" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>COMPOSIÇÃO DO SALDO ATUAL DO ESTOQUE</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1639,17 +1913,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F6" totalsRowCount="1" headerRowDxfId="45" totalsRowDxfId="44">
-  <autoFilter ref="A3:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TblCadastro" displayName="TblCadastro" ref="A3:F12" totalsRowCount="1" headerRowDxfId="27" dataDxfId="26" totalsRowDxfId="25">
+  <autoFilter ref="A3:F11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="26"/>
-    <tableColumn id="2" name="MEDIDA" totalsRowDxfId="25"/>
-    <tableColumn id="3" name="ESTOQUE MÍNIMO" totalsRowDxfId="24"/>
-    <tableColumn id="4" name="ESTOQUE MÁXIMO" totalsRowDxfId="23"/>
-    <tableColumn id="5" name="SALDO" dataDxfId="43" totalsRowDxfId="22">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="2" name="MEDIDA" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="3" name="ESTOQUE MÍNIMO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="4" name="ESTOQUE MÁXIMO" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="AVISOS" totalsRowFunction="count" dataDxfId="42" totalsRowDxfId="21">
+    <tableColumn id="6" name="AVISOS" dataDxfId="14" totalsRowDxfId="13">
       <calculatedColumnFormula>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1658,14 +1932,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E8" totalsRowCount="1" headerRowDxfId="19" totalsRowDxfId="18">
-  <autoFilter ref="A3:E7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TblLancamentos" displayName="TblLancamentos" ref="A3:E108" totalsRowCount="1" headerRowDxfId="10" totalsRowDxfId="9">
+  <autoFilter ref="A3:E107"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="DATA" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="10"/>
-    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="9"/>
-    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="8"/>
-    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="7">
+    <tableColumn id="1" name="PRODUTO" totalsRowLabel="Total" totalsRowDxfId="8"/>
+    <tableColumn id="2" name="DATA" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" name="ENTRADA" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="SAÍDA" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="SALDO" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1962,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,7 +2251,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1985,115 +2259,251 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="60.7109375" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="40.7109375" style="13" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="13" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="13">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13">
         <v>150</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="10">
         <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
-        <v>998</v>
-      </c>
-      <c r="F4" s="1" t="str">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="13">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13">
+        <v>150</v>
+      </c>
+      <c r="E5" s="10">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>11</v>
+      </c>
+      <c r="F5" s="10" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v>Solicitar nova compra!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13">
+        <v>30</v>
+      </c>
+      <c r="D6" s="13">
+        <v>150</v>
+      </c>
+      <c r="E6" s="14">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>22</v>
+      </c>
+      <c r="F6" s="14" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v>Solicitar nova compra!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13">
+        <v>10</v>
+      </c>
+      <c r="D7" s="13">
+        <v>50</v>
+      </c>
+      <c r="E7" s="14">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>35</v>
+      </c>
+      <c r="F7" s="14" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="13">
+        <v>20</v>
+      </c>
+      <c r="D8" s="13">
+        <v>250</v>
+      </c>
+      <c r="E8" s="14">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>56</v>
+      </c>
+      <c r="F8" s="14" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13">
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <v>25</v>
+      </c>
+      <c r="E9" s="14">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>64</v>
+      </c>
+      <c r="F9" s="14" t="str">
         <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
         <v>Priorizar venda!</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>150</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C10" s="13">
+        <v>5</v>
+      </c>
+      <c r="D10" s="13">
+        <v>25</v>
+      </c>
+      <c r="E10" s="14">
         <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
-        <v>-9952</v>
-      </c>
-      <c r="F5" s="1" t="str">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14" t="str">
         <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
-        <v>Solicitar nova compra!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="13">
+        <v>5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>30</v>
+      </c>
+      <c r="E11" s="14">
+        <f>SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[ENTRADA])-SUMIF(TblLancamentos[PRODUTO],TblCadastro[[#This Row],[PRODUTO]],TblLancamentos[SAÍDA])</f>
+        <v>30</v>
+      </c>
+      <c r="F11" s="14" t="str">
+        <f>IF(TblCadastro[[#This Row],[SALDO]]&lt;TblCadastro[[#This Row],[ESTOQUE MÍNIMO]],"Solicitar nova compra!",IF(TblCadastro[[#This Row],[SALDO]]&gt;TblCadastro[[#This Row],[ESTOQUE MÁXIMO]],"Priorizar venda!",""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <f>SUBTOTAL(103,TblCadastro[AVISOS])</f>
-        <v>2</v>
-      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
+        <f>SUBTOTAL(109,TblCadastro[SALDO])</f>
+        <v>263</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:D5">
-    <cfRule type="expression" dxfId="4" priority="7">
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <conditionalFormatting sqref="A4:D11">
+    <cfRule type="expression" dxfId="30" priority="7">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="F4:F11">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"Priorizar venda!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"Solicitar nova compra!"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D5">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D11">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
     </dataValidation>
@@ -2109,10 +2519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,10 +2542,10 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -2144,118 +2554,1915 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4">
-        <v>43698</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="5">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6">
-        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>988</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43106</v>
+      </c>
+      <c r="C4" s="4">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>43699</v>
-      </c>
-      <c r="C5" s="5">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6">
-        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>998</v>
+      <c r="B5" s="3">
+        <v>43104</v>
+      </c>
+      <c r="C5" s="4">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
-        <v>43605</v>
-      </c>
-      <c r="C6" s="5">
-        <v>50</v>
-      </c>
-      <c r="D6" s="5">
-        <v>10000</v>
-      </c>
-      <c r="E6" s="6">
-        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>-9952</v>
+      <c r="B6" s="3">
+        <v>43105</v>
+      </c>
+      <c r="C6" s="4">
+        <v>78</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43102</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43116</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
-        <v>43497</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="E8" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43129</v>
+      </c>
+      <c r="C9" s="4">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>43136</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3">
+        <v>43136</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43141</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43143</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>43145</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>43146</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3">
+        <v>43153</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <v>43157</v>
+      </c>
+      <c r="C17" s="4">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3">
+        <v>43158</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
         <v>10</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E18" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43162</v>
+      </c>
+      <c r="C19" s="4">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43166</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
+        <v>43167</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3">
+        <v>43169</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6</v>
+      </c>
+      <c r="E22" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>43170</v>
+      </c>
+      <c r="C23" s="4">
+        <v>20</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3">
+        <v>43173</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3">
+        <v>43174</v>
+      </c>
+      <c r="C25" s="4">
+        <v>29</v>
+      </c>
+      <c r="D25" s="4">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3">
+        <v>43175</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>6</v>
+      </c>
+      <c r="E26" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3">
+        <v>43177</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="3">
+        <v>43180</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="3">
+        <v>43181</v>
+      </c>
+      <c r="C29" s="4">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3">
+        <v>43182</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>7</v>
+      </c>
+      <c r="E30" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3">
+        <v>43186</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3">
+        <v>43186</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="3">
+        <v>43198</v>
+      </c>
+      <c r="C33" s="4">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4">
+        <v>8</v>
+      </c>
+      <c r="E33" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3">
+        <v>43203</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>6</v>
+      </c>
+      <c r="E34" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="3">
+        <v>43204</v>
+      </c>
+      <c r="C35" s="4">
+        <v>22</v>
+      </c>
+      <c r="D35" s="4">
+        <v>9</v>
+      </c>
+      <c r="E35" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="3">
+        <v>43212</v>
+      </c>
+      <c r="C36" s="4">
+        <v>22</v>
+      </c>
+      <c r="D36" s="4">
+        <v>7</v>
+      </c>
+      <c r="E36" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="3">
+        <v>43217</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="3">
+        <v>43221</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>7</v>
+      </c>
+      <c r="E38" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="3">
+        <v>43222</v>
+      </c>
+      <c r="C39" s="4">
+        <v>31</v>
+      </c>
+      <c r="D39" s="4">
+        <v>8</v>
+      </c>
+      <c r="E39" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>9</v>
+      </c>
+      <c r="E40" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="3">
+        <v>43231</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>9</v>
+      </c>
+      <c r="E41" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3">
+        <v>43231</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+      <c r="D42" s="4">
+        <v>8</v>
+      </c>
+      <c r="E42" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43235</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>5</v>
+      </c>
+      <c r="E43" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43235</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>8</v>
+      </c>
+      <c r="E44" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <v>9</v>
+      </c>
+      <c r="E45" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
+        <v>7</v>
+      </c>
+      <c r="E46" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>9</v>
+      </c>
+      <c r="E47" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="3">
+        <v>43239</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <v>7</v>
+      </c>
+      <c r="E48" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="3">
+        <v>43240</v>
+      </c>
+      <c r="C49" s="4">
+        <v>24</v>
+      </c>
+      <c r="D49" s="4">
+        <v>5</v>
+      </c>
+      <c r="E49" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="3">
+        <v>43242</v>
+      </c>
+      <c r="C50" s="4">
+        <v>10</v>
+      </c>
+      <c r="D50" s="4">
+        <v>10</v>
+      </c>
+      <c r="E50" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="3">
+        <v>43244</v>
+      </c>
+      <c r="C51" s="4">
+        <v>2</v>
+      </c>
+      <c r="D51" s="4">
+        <v>6</v>
+      </c>
+      <c r="E51" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="3">
+        <v>43248</v>
+      </c>
+      <c r="C52" s="4">
+        <v>27</v>
+      </c>
+      <c r="D52" s="4">
+        <v>10</v>
+      </c>
+      <c r="E52" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="3">
+        <v>43253</v>
+      </c>
+      <c r="C53" s="4">
+        <v>9</v>
+      </c>
+      <c r="D53" s="4">
+        <v>5</v>
+      </c>
+      <c r="E53" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="3">
+        <v>43265</v>
+      </c>
+      <c r="C54" s="4">
+        <v>17</v>
+      </c>
+      <c r="D54" s="4">
+        <v>5</v>
+      </c>
+      <c r="E54" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="3">
+        <v>43267</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0</v>
+      </c>
+      <c r="D55" s="4">
+        <v>6</v>
+      </c>
+      <c r="E55" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="3">
+        <v>43273</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4">
+        <v>10</v>
+      </c>
+      <c r="E56" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="3">
+        <v>43273</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4">
+        <v>9</v>
+      </c>
+      <c r="E57" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="3">
+        <v>43278</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
+      <c r="D58" s="4">
+        <v>5</v>
+      </c>
+      <c r="E58" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="3">
+        <v>43290</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
+      <c r="D59" s="4">
+        <v>9</v>
+      </c>
+      <c r="E59" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="3">
+        <v>43299</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
+      <c r="D60" s="4">
+        <v>6</v>
+      </c>
+      <c r="E60" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="3">
+        <v>43305</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0</v>
+      </c>
+      <c r="D61" s="4">
+        <v>9</v>
+      </c>
+      <c r="E61" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="3">
+        <v>43312</v>
+      </c>
+      <c r="C62" s="4">
+        <v>8</v>
+      </c>
+      <c r="D62" s="4">
+        <v>7</v>
+      </c>
+      <c r="E62" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="3">
+        <v>43317</v>
+      </c>
+      <c r="C63" s="4">
+        <v>24</v>
+      </c>
+      <c r="D63" s="4">
+        <v>8</v>
+      </c>
+      <c r="E63" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="3">
+        <v>43318</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0</v>
+      </c>
+      <c r="D64" s="4">
+        <v>5</v>
+      </c>
+      <c r="E64" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="3">
+        <v>43319</v>
+      </c>
+      <c r="C65" s="4">
+        <v>25</v>
+      </c>
+      <c r="D65" s="4">
+        <v>10</v>
+      </c>
+      <c r="E65" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="3">
+        <v>43328</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0</v>
+      </c>
+      <c r="D66" s="4">
+        <v>10</v>
+      </c>
+      <c r="E66" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="3">
+        <v>43328</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0</v>
+      </c>
+      <c r="D67" s="4">
+        <v>8</v>
+      </c>
+      <c r="E67" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="3">
+        <v>43329</v>
+      </c>
+      <c r="C68" s="4">
+        <v>3</v>
+      </c>
+      <c r="D68" s="4">
+        <v>7</v>
+      </c>
+      <c r="E68" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="3">
+        <v>43329</v>
+      </c>
+      <c r="C69" s="4">
+        <v>26</v>
+      </c>
+      <c r="D69" s="4">
+        <v>10</v>
+      </c>
+      <c r="E69" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="3">
+        <v>43330</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0</v>
+      </c>
+      <c r="D70" s="4">
+        <v>8</v>
+      </c>
+      <c r="E70" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="3">
+        <v>43331</v>
+      </c>
+      <c r="C71" s="4">
+        <v>5</v>
+      </c>
+      <c r="D71" s="4">
+        <v>8</v>
+      </c>
+      <c r="E71" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="3">
+        <v>43333</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <v>6</v>
+      </c>
+      <c r="E72" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="3">
+        <v>43336</v>
+      </c>
+      <c r="C73" s="4">
+        <v>0</v>
+      </c>
+      <c r="D73" s="4">
+        <v>6</v>
+      </c>
+      <c r="E73" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="3">
+        <v>43337</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0</v>
+      </c>
+      <c r="D74" s="4">
+        <v>9</v>
+      </c>
+      <c r="E74" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="3">
+        <v>43338</v>
+      </c>
+      <c r="C75" s="4">
+        <v>25</v>
+      </c>
+      <c r="D75" s="4">
+        <v>6</v>
+      </c>
+      <c r="E75" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="3">
+        <v>43342</v>
+      </c>
+      <c r="C76" s="4">
+        <v>0</v>
+      </c>
+      <c r="D76" s="4">
+        <v>7</v>
+      </c>
+      <c r="E76" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>15</v>
+      </c>
+      <c r="B77" s="3">
+        <v>43344</v>
+      </c>
+      <c r="C77" s="4">
+        <v>0</v>
+      </c>
+      <c r="D77" s="4">
+        <v>7</v>
+      </c>
+      <c r="E77" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="3">
+        <v>43353</v>
+      </c>
+      <c r="C78" s="4">
+        <v>0</v>
+      </c>
+      <c r="D78" s="4">
+        <v>8</v>
+      </c>
+      <c r="E78" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" s="3">
+        <v>43359</v>
+      </c>
+      <c r="C79" s="4">
+        <v>29</v>
+      </c>
+      <c r="D79" s="4">
+        <v>5</v>
+      </c>
+      <c r="E79" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>17</v>
+      </c>
+      <c r="B80" s="3">
+        <v>43367</v>
+      </c>
+      <c r="C80" s="4">
+        <v>32</v>
+      </c>
+      <c r="D80" s="4">
+        <v>6</v>
+      </c>
+      <c r="E80" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="3">
+        <v>43368</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0</v>
+      </c>
+      <c r="D81" s="4">
+        <v>6</v>
+      </c>
+      <c r="E81" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="3">
+        <v>43371</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0</v>
+      </c>
+      <c r="D82" s="4">
+        <v>7</v>
+      </c>
+      <c r="E82" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="3">
+        <v>43377</v>
+      </c>
+      <c r="C83" s="4">
+        <v>17</v>
+      </c>
+      <c r="D83" s="4">
+        <v>7</v>
+      </c>
+      <c r="E83" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="3">
+        <v>43379</v>
+      </c>
+      <c r="C84" s="4">
+        <v>24</v>
+      </c>
+      <c r="D84" s="4">
+        <v>5</v>
+      </c>
+      <c r="E84" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
         <v>12</v>
       </c>
-      <c r="E7" s="6">
-        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="3">
+        <v>43383</v>
+      </c>
+      <c r="C85" s="4">
+        <v>0</v>
+      </c>
+      <c r="D85" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <f>SUBTOTAL(103,TblLancamentos[DATA])</f>
+      <c r="E85" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="3">
+        <v>43387</v>
+      </c>
+      <c r="C86" s="4">
+        <v>0</v>
+      </c>
+      <c r="D86" s="4">
+        <v>7</v>
+      </c>
+      <c r="E86" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B87" s="3">
+        <v>43390</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0</v>
+      </c>
+      <c r="D87" s="4">
+        <v>9</v>
+      </c>
+      <c r="E87" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="3">
+        <v>43391</v>
+      </c>
+      <c r="C88" s="4">
+        <v>0</v>
+      </c>
+      <c r="D88" s="4">
+        <v>6</v>
+      </c>
+      <c r="E88" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6">
+      <c r="B89" s="3">
+        <v>43394</v>
+      </c>
+      <c r="C89" s="4">
+        <v>0</v>
+      </c>
+      <c r="D89" s="4">
+        <v>9</v>
+      </c>
+      <c r="E89" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="3">
+        <v>43395</v>
+      </c>
+      <c r="C90" s="4">
+        <v>0</v>
+      </c>
+      <c r="D90" s="4">
+        <v>10</v>
+      </c>
+      <c r="E90" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="3">
+        <v>43396</v>
+      </c>
+      <c r="C91" s="4">
+        <v>0</v>
+      </c>
+      <c r="D91" s="4">
+        <v>5</v>
+      </c>
+      <c r="E91" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" s="3">
+        <v>43399</v>
+      </c>
+      <c r="C92" s="4">
+        <v>30</v>
+      </c>
+      <c r="D92" s="4">
+        <v>9</v>
+      </c>
+      <c r="E92" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="3">
+        <v>43401</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0</v>
+      </c>
+      <c r="D93" s="4">
+        <v>9</v>
+      </c>
+      <c r="E93" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" s="3">
+        <v>43403</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0</v>
+      </c>
+      <c r="D94" s="4">
+        <v>5</v>
+      </c>
+      <c r="E94" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" s="3">
+        <v>43404</v>
+      </c>
+      <c r="C95" s="4">
+        <v>0</v>
+      </c>
+      <c r="D95" s="4">
+        <v>7</v>
+      </c>
+      <c r="E95" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>13</v>
+      </c>
+      <c r="B96" s="3">
+        <v>43410</v>
+      </c>
+      <c r="C96" s="4">
+        <v>0</v>
+      </c>
+      <c r="D96" s="4">
+        <v>8</v>
+      </c>
+      <c r="E96" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="3">
+        <v>43415</v>
+      </c>
+      <c r="C97" s="4">
+        <v>25</v>
+      </c>
+      <c r="D97" s="4">
+        <v>0</v>
+      </c>
+      <c r="E97" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98" s="3">
+        <v>43415</v>
+      </c>
+      <c r="C98" s="4">
+        <v>15</v>
+      </c>
+      <c r="D98" s="4">
+        <v>0</v>
+      </c>
+      <c r="E98" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="3">
+        <v>43415</v>
+      </c>
+      <c r="C99" s="4">
+        <v>35</v>
+      </c>
+      <c r="D99" s="4">
+        <v>0</v>
+      </c>
+      <c r="E99" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>15</v>
+      </c>
+      <c r="B100" s="3">
+        <v>43415</v>
+      </c>
+      <c r="C100" s="4">
+        <v>80</v>
+      </c>
+      <c r="D100" s="4">
+        <v>0</v>
+      </c>
+      <c r="E100" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="3">
+        <v>43416</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+      <c r="D101" s="4">
+        <v>25</v>
+      </c>
+      <c r="E101" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="3">
+        <v>43416</v>
+      </c>
+      <c r="C102" s="4">
+        <v>0</v>
+      </c>
+      <c r="D102" s="4">
+        <v>25</v>
+      </c>
+      <c r="E102" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" s="3">
+        <v>43419</v>
+      </c>
+      <c r="C103" s="4">
+        <v>45</v>
+      </c>
+      <c r="D103" s="4">
+        <v>0</v>
+      </c>
+      <c r="E103" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="3">
+        <v>43419</v>
+      </c>
+      <c r="C104" s="4">
+        <v>28</v>
+      </c>
+      <c r="D104" s="4">
+        <v>0</v>
+      </c>
+      <c r="E104" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>19</v>
+      </c>
+      <c r="B105" s="3">
+        <v>43419</v>
+      </c>
+      <c r="C105" s="4">
+        <v>24</v>
+      </c>
+      <c r="D105" s="4">
+        <v>0</v>
+      </c>
+      <c r="E105" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106" s="3">
+        <v>43420</v>
+      </c>
+      <c r="C106" s="4">
+        <v>0</v>
+      </c>
+      <c r="D106" s="4">
+        <v>6</v>
+      </c>
+      <c r="E106" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" s="3">
+        <v>43790</v>
+      </c>
+      <c r="C107" s="4">
+        <v>40</v>
+      </c>
+      <c r="D107" s="4">
+        <v>5</v>
+      </c>
+      <c r="E107" s="5">
+        <f>SUMIFS(TblLancamentos[ENTRADA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])-SUMIFS(TblLancamentos[SAÍDA],TblLancamentos[PRODUTO],TblLancamentos[[#This Row],[PRODUTO]],TblLancamentos[DATA],"&lt;="&amp;TblLancamentos[[#This Row],[DATA]])</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8">
         <f>SUBTOTAL(109,TblLancamentos[ENTRADA])</f>
-        <v>1080</v>
-      </c>
-      <c r="D8" s="6">
+        <v>1005</v>
+      </c>
+      <c r="D108" s="8">
         <f>SUBTOTAL(109,TblLancamentos[SAÍDA])</f>
-        <v>10034</v>
-      </c>
-      <c r="E8" s="1">
+        <v>742</v>
+      </c>
+      <c r="E108" s="8">
         <f>SUBTOTAL(103,TblLancamentos[SALDO])</f>
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:D7">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A4:D107">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>ODD(ROW())=ROW()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E7">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="E4:E107">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B7">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Por favor_x000a__x000a_Digite uma data válida_x000a__x000a_Ex: 04/05/2020" sqref="B4:B107">
       <formula1>1</formula1>
       <formula2>401769</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D107">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A107">
       <formula1>ColunaProdutos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>